<commit_message>
Updated data, work on analysis of new data
</commit_message>
<xml_diff>
--- a/Fig. 4_Primary data_OB.xlsx
+++ b/Fig. 4_Primary data_OB.xlsx
@@ -5,15 +5,17 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pospij\Desktop\publikační snímky\PRO OB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pospij\Desktop\publikační snímky\PRIMARY DATA\Fig. 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Fig.4 chart b" sheetId="8" r:id="rId1"/>
-    <sheet name="Fig.4 chart c" sheetId="9" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="10" r:id="rId1"/>
+    <sheet name="Fig.4 chart b" sheetId="8" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="11" r:id="rId3"/>
+    <sheet name="Fig.4 chart c" sheetId="9" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="60">
   <si>
     <t>1925+2380</t>
   </si>
@@ -84,17 +86,134 @@
     <t>hs-comK</t>
   </si>
   <si>
-    <t>comK</t>
-  </si>
-  <si>
     <t>qPCR results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wt </t>
+  </si>
+  <si>
+    <t>SigD</t>
+  </si>
+  <si>
+    <t>SigD+Dnase</t>
+  </si>
+  <si>
+    <t>Wt+DNase</t>
+  </si>
+  <si>
+    <t>comK UP</t>
+  </si>
+  <si>
+    <t>comK UP + Dnase</t>
+  </si>
+  <si>
+    <t>comk</t>
+  </si>
+  <si>
+    <t>comk+Dnase</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>Column3</t>
+  </si>
+  <si>
+    <t>Column4</t>
+  </si>
+  <si>
+    <t>Column5</t>
+  </si>
+  <si>
+    <t>Column6</t>
+  </si>
+  <si>
+    <t>Column7</t>
+  </si>
+  <si>
+    <t>Column8</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Standard Error</t>
+  </si>
+  <si>
+    <t>Median</t>
+  </si>
+  <si>
+    <t>Mode</t>
+  </si>
+  <si>
+    <t>Standard Deviation</t>
+  </si>
+  <si>
+    <t>Sample Variance</t>
+  </si>
+  <si>
+    <t>Kurtosis</t>
+  </si>
+  <si>
+    <t>Skewness</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>Minimum</t>
+  </si>
+  <si>
+    <t>Maximum</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Wt</t>
+  </si>
+  <si>
+    <t>Wt + DNase</t>
+  </si>
+  <si>
+    <t>SigD + DNase</t>
+  </si>
+  <si>
+    <t>ComKUP</t>
+  </si>
+  <si>
+    <t>ComKUP+DNase</t>
+  </si>
+  <si>
+    <t>comKKO</t>
+  </si>
+  <si>
+    <t>comKKO+DNase</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>KOcomK</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>SEM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,6 +237,15 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -158,7 +286,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -261,11 +389,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -282,6 +421,17 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -562,10 +712,727 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AR10"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AJ16" sqref="AJ16"/>
+      <selection activeCell="P4" activeCellId="7" sqref="B4 D4 F4 H4 J4 L4 N4 P4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="P1" s="19"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="17">
+        <v>4.9402713618409448E-3</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="17">
+        <v>0</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="17">
+        <v>9.434762544374872E-4</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="17">
+        <v>0</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="17">
+        <v>2.2974371785696106</v>
+      </c>
+      <c r="K3" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" s="17">
+        <v>0</v>
+      </c>
+      <c r="M3" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="17">
+        <v>0</v>
+      </c>
+      <c r="O3" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="P3" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="17">
+        <v>5.0616713556736058E-4</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="17">
+        <v>0</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="17">
+        <v>1.1057554551586095E-4</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="17">
+        <v>0</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" s="17">
+        <v>0.49968109994353971</v>
+      </c>
+      <c r="K4" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="L4" s="17">
+        <v>0</v>
+      </c>
+      <c r="M4" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="N4" s="17">
+        <v>0</v>
+      </c>
+      <c r="O4" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="P4" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="17">
+        <v>5.2245862884160756E-3</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="17">
+        <v>0</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="17">
+        <v>9.2150170648464165E-4</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="17">
+        <v>0</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" s="17">
+        <v>2.0134228187919465</v>
+      </c>
+      <c r="K5" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="L5" s="17">
+        <v>0</v>
+      </c>
+      <c r="M5" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="N5" s="17">
+        <v>0</v>
+      </c>
+      <c r="O5" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="P5" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="17" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="17">
+        <v>0</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="17" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="17">
+        <v>0</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" s="17" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K6" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="L6" s="17">
+        <v>0</v>
+      </c>
+      <c r="M6" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="N6" s="17">
+        <v>0</v>
+      </c>
+      <c r="O6" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="P6" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="17">
+        <v>8.7670719592427226E-4</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="17">
+        <v>0</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="17">
+        <v>1.915224629081161E-4</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="17">
+        <v>0</v>
+      </c>
+      <c r="I7" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="J7" s="17">
+        <v>0.86547305268411279</v>
+      </c>
+      <c r="K7" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="L7" s="17">
+        <v>0</v>
+      </c>
+      <c r="M7" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="N7" s="17">
+        <v>0</v>
+      </c>
+      <c r="O7" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="P7" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="17">
+        <v>7.6861550738540038E-7</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="17">
+        <v>0</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="17">
+        <v>3.6680853798390709E-8</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="17">
+        <v>0</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="J8" s="17">
+        <v>0.749043604922357</v>
+      </c>
+      <c r="K8" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="L8" s="17">
+        <v>0</v>
+      </c>
+      <c r="M8" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="N8" s="17">
+        <v>0</v>
+      </c>
+      <c r="O8" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="P8" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="17" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="17" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="17" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" s="17" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" s="17" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K9" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="L9" s="17" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M9" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="N9" s="17" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O9" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="P9" s="17" t="e">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="17">
+        <v>-1.3058651694147949</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="17" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="17">
+        <v>0.50951568968611705</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" s="17" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="J10" s="17">
+        <v>1.317696065246289</v>
+      </c>
+      <c r="K10" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="L10" s="17" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M10" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="N10" s="17" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O10" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="P10" s="17" t="e">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="17">
+        <v>1.682841970335104E-3</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="17">
+        <v>0</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="17">
+        <v>3.8114927905004241E-4</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11" s="17">
+        <v>0</v>
+      </c>
+      <c r="I11" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="J11" s="17">
+        <v>1.6595728215446524</v>
+      </c>
+      <c r="K11" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="L11" s="17">
+        <v>0</v>
+      </c>
+      <c r="M11" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="N11" s="17">
+        <v>0</v>
+      </c>
+      <c r="O11" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="P11" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="17">
+        <v>3.9566929133858265E-3</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="17">
+        <v>0</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="17">
+        <v>7.6388888888888893E-4</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="H12" s="17">
+        <v>0</v>
+      </c>
+      <c r="I12" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="J12" s="17">
+        <v>1.6096579476861168</v>
+      </c>
+      <c r="K12" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="L12" s="17">
+        <v>0</v>
+      </c>
+      <c r="M12" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="N12" s="17">
+        <v>0</v>
+      </c>
+      <c r="O12" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="P12" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="17">
+        <v>5.6395348837209305E-3</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="17">
+        <v>0</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="17">
+        <v>1.1450381679389313E-3</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" s="17">
+        <v>0</v>
+      </c>
+      <c r="I13" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="J13" s="17">
+        <v>3.2692307692307692</v>
+      </c>
+      <c r="K13" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="L13" s="17">
+        <v>0</v>
+      </c>
+      <c r="M13" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="N13" s="17">
+        <v>0</v>
+      </c>
+      <c r="O13" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="P13" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="17">
+        <v>1.4820814085522833E-2</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="17">
+        <v>0</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="17">
+        <v>2.8304287633124617E-3</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="H14" s="17">
+        <v>0</v>
+      </c>
+      <c r="I14" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="J14" s="17">
+        <v>6.8923115357088323</v>
+      </c>
+      <c r="K14" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="L14" s="17">
+        <v>0</v>
+      </c>
+      <c r="M14" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="N14" s="17">
+        <v>0</v>
+      </c>
+      <c r="O14" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="P14" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="18">
+        <v>3</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="18">
+        <v>3</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" s="18">
+        <v>3</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="H15" s="18">
+        <v>3</v>
+      </c>
+      <c r="I15" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="J15" s="18">
+        <v>3</v>
+      </c>
+      <c r="K15" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="L15" s="18">
+        <v>3</v>
+      </c>
+      <c r="M15" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="N15" s="18">
+        <v>3</v>
+      </c>
+      <c r="O15" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="P15" s="18">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AR40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1237,25 +2104,665 @@
       </c>
       <c r="AR10" s="2"/>
     </row>
+    <row r="12" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" t="s">
+        <v>25</v>
+      </c>
+      <c r="I12" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="C13" s="16">
+        <v>5.2245862884160756E-3</v>
+      </c>
+      <c r="D13" s="16">
+        <v>0</v>
+      </c>
+      <c r="E13" s="16">
+        <v>7.6388888888888893E-4</v>
+      </c>
+      <c r="F13" s="16">
+        <v>0</v>
+      </c>
+      <c r="G13" s="16">
+        <v>1.6096579476861168</v>
+      </c>
+      <c r="H13" s="16">
+        <v>0</v>
+      </c>
+      <c r="I13" s="16">
+        <v>0</v>
+      </c>
+      <c r="J13" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="C14" s="16">
+        <v>5.6395348837209305E-3</v>
+      </c>
+      <c r="D14" s="16">
+        <v>0</v>
+      </c>
+      <c r="E14" s="16">
+        <v>1.1450381679389313E-3</v>
+      </c>
+      <c r="F14" s="16">
+        <v>0</v>
+      </c>
+      <c r="G14" s="16">
+        <v>2.0134228187919465</v>
+      </c>
+      <c r="H14" s="16">
+        <v>0</v>
+      </c>
+      <c r="I14" s="16">
+        <v>0</v>
+      </c>
+      <c r="J14" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="C15" s="16">
+        <v>3.9566929133858265E-3</v>
+      </c>
+      <c r="D15" s="16">
+        <v>0</v>
+      </c>
+      <c r="E15" s="16">
+        <v>9.2150170648464165E-4</v>
+      </c>
+      <c r="F15" s="16">
+        <v>0</v>
+      </c>
+      <c r="G15" s="16">
+        <v>3.2692307692307692</v>
+      </c>
+      <c r="H15" s="16">
+        <v>0</v>
+      </c>
+      <c r="I15" s="16">
+        <v>0</v>
+      </c>
+      <c r="J15" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="20">
+        <v>4.9402713618409448E-3</v>
+      </c>
+      <c r="D16" s="20">
+        <v>0</v>
+      </c>
+      <c r="E16" s="20">
+        <v>9.434762544374872E-4</v>
+      </c>
+      <c r="F16" s="20">
+        <v>0</v>
+      </c>
+      <c r="G16" s="20">
+        <v>2.2974371785696106</v>
+      </c>
+      <c r="H16" s="20">
+        <v>0</v>
+      </c>
+      <c r="I16" s="20">
+        <v>0</v>
+      </c>
+      <c r="J16" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="17">
+        <v>5.0616713556736058E-4</v>
+      </c>
+      <c r="D17" s="17">
+        <v>0</v>
+      </c>
+      <c r="E17" s="17">
+        <v>1.1057554551586095E-4</v>
+      </c>
+      <c r="F17" s="17">
+        <v>0</v>
+      </c>
+      <c r="G17" s="17">
+        <v>0.49968109994353971</v>
+      </c>
+      <c r="H17" s="17">
+        <v>0</v>
+      </c>
+      <c r="I17" s="17">
+        <v>0</v>
+      </c>
+      <c r="J17" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J26" s="21"/>
+      <c r="L26" s="21"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J27" s="21"/>
+      <c r="L27" s="21"/>
+    </row>
+    <row r="33" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E33" t="s">
+        <v>49</v>
+      </c>
+      <c r="F33" s="21">
+        <v>4.9402999999999999E-3</v>
+      </c>
+      <c r="G33" s="21">
+        <v>5.0617000000000001E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E34" t="s">
+        <v>50</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E35" t="s">
+        <v>21</v>
+      </c>
+      <c r="F35" s="21">
+        <v>9.4348000000000001E-4</v>
+      </c>
+      <c r="G35" s="21">
+        <v>1.1058E-4</v>
+      </c>
+    </row>
+    <row r="36" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E36" t="s">
+        <v>51</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E37" t="s">
+        <v>52</v>
+      </c>
+      <c r="F37">
+        <v>2.2974000000000001</v>
+      </c>
+      <c r="G37">
+        <v>0.49969999999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E38" t="s">
+        <v>53</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E39" t="s">
+        <v>54</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E40" t="s">
+        <v>55</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="19"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="17">
+        <v>100</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="17">
+        <v>40.09737700682205</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="17">
+        <v>8468.8369463166655</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="17">
+        <v>0.10752760937202203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="17">
+        <v>0</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="17">
+        <v>6.1950325316115462</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="17">
+        <v>1676.5184974646234</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="17">
+        <v>7.5724989987208752E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="17">
+        <v>100</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="17">
+        <v>45.800053758496716</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="17">
+        <v>9488.9429999999993</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="17">
+        <v>5.2208734262937088E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="17">
+        <v>100</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="17" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="17" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="17" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="17">
+        <v>0</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="17">
+        <v>10.730111099293245</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="17">
+        <v>2903.8152174377615</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="17">
+        <v>0.13115953006049005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="17">
+        <v>0</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="17">
+        <v>115.13528420317607</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="17">
+        <v>8432142.8170231134</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="17">
+        <v>1.7202822325688594E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="17" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="17" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="17" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" s="17" t="e">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="17" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="17">
+        <v>-1.7160750182423441</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="17">
+        <v>-1.3857504994882179</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" s="17">
+        <v>1.560331655467142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="17">
+        <v>0</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="17">
+        <v>19.05202273803058</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="17">
+        <v>5532.3342438620148</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11" s="17">
+        <v>0.24419409385312901</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="17">
+        <v>100</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="17">
+        <v>27.72002726196942</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="17">
+        <v>5192.6167975439912</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="H12" s="17">
+        <v>1.3089999999999999E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="17">
+        <v>100</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="17">
+        <v>46.77205</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="17">
+        <v>10724.951041406006</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" s="17">
+        <v>0.257284093853129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="17">
+        <v>300</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="17">
+        <v>120.29213102046614</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="17">
+        <v>25406.510838949995</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="H14" s="17">
+        <v>0.32258282811606609</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="18">
+        <v>3</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="18">
+        <v>3</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" s="18">
+        <v>3</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="H15" s="18">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W34" sqref="W34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="12"/>
@@ -1269,59 +2776,109 @@
         <v>18</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C2" s="13" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D2" s="14">
         <v>100</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="23">
         <v>45.800053758496716</v>
       </c>
       <c r="F2" s="14">
-        <v>1766.8041959807294</v>
+        <v>5192.6167975439912</v>
       </c>
       <c r="G2" s="14">
-        <v>7.6394906645295496E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>5.2208734262937088E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C3" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="14">
+        <v>5</v>
+      </c>
+      <c r="D3" s="15">
         <v>100</v>
       </c>
       <c r="E3" s="15">
         <v>27.72002726196942</v>
       </c>
-      <c r="F3" s="14">
-        <v>5192.6167975439912</v>
-      </c>
-      <c r="G3" s="14">
-        <v>5.2208734262937088E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F3" s="15">
+        <v>10724.951041406006</v>
+      </c>
+      <c r="G3" s="15">
+        <v>0.257284093853129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C4" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="15">
+        <v>58</v>
+      </c>
+      <c r="D4" s="24">
         <v>100</v>
       </c>
-      <c r="E4" s="14">
-        <v>47.744987887915634</v>
-      </c>
-      <c r="F4" s="15">
-        <v>10724.951041406006</v>
-      </c>
-      <c r="G4" s="15">
-        <v>0.257284093853129</v>
-      </c>
+      <c r="E4" s="24">
+        <v>46.77205</v>
+      </c>
+      <c r="F4" s="24">
+        <v>9488.9429999999993</v>
+      </c>
+      <c r="G4" s="24">
+        <v>1.3089999999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C5" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="17">
+        <v>100</v>
+      </c>
+      <c r="E5" s="17">
+        <v>40.09737700682205</v>
+      </c>
+      <c r="F5" s="17">
+        <v>8468.8369463166655</v>
+      </c>
+      <c r="G5" s="17">
+        <v>0.10752760937202203</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C6" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="17">
+        <v>0</v>
+      </c>
+      <c r="E6" s="17">
+        <v>6.1950325316115462</v>
+      </c>
+      <c r="F6" s="17">
+        <v>1676.5184974646234</v>
+      </c>
+      <c r="G6" s="17">
+        <v>7.5724989987208752E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="O14" s="17"/>
+      <c r="P14" s="17"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="O15" s="17"/>
+      <c r="P15" s="17"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
+    </row>
+    <row r="17" spans="15:16" x14ac:dyDescent="0.3">
+      <c r="O17" s="17"/>
+      <c r="P17" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>